<commit_message>
Changed data types chart to show # files instead of size. Protected all worksheets and workbook (no password)
</commit_message>
<xml_diff>
--- a/exceltemplate/lightgrep_Search_Report.xlsx
+++ b/exceltemplate/lightgrep_Search_Report.xlsx
@@ -3,6 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <workbookProtection lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="20295" windowHeight="6345"/>
   </bookViews>
@@ -17,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="235">
   <si>
     <t>Keyword Name</t>
   </si>
@@ -706,9 +707,6 @@
     <t>Hits % of Total</t>
   </si>
   <si>
-    <t>Grand Total (All Keywords))</t>
-  </si>
-  <si>
     <t>Top Ten By File Type</t>
   </si>
   <si>
@@ -719,6 +717,12 @@
   </si>
   <si>
     <t>% of Total Size</t>
+  </si>
+  <si>
+    <t>Grand Total (All Types)</t>
+  </si>
+  <si>
+    <t>Grand Total (All Keywords)</t>
   </si>
 </sst>
 </file>
@@ -726,7 +730,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="#,##0&quot; MB&quot;"/>
+    <numFmt numFmtId="164" formatCode="#,##0&quot; MB&quot;"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -789,11 +793,11 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -869,10 +873,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="2.6931218110854846E-2"/>
-          <c:y val="0.11528964233199339"/>
+          <c:x val="2.6931218110854863E-2"/>
+          <c:y val="0.11528964233199342"/>
           <c:w val="0.92562552056694924"/>
-          <c:h val="0.78358330447699776"/>
+          <c:h val="0.78358330447699742"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -1001,24 +1005,25 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:gapWidth val="100"/>
-        <c:axId val="109515520"/>
-        <c:axId val="109517056"/>
+        <c:axId val="77584256"/>
+        <c:axId val="83606528"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="109515520"/>
+        <c:axId val="77584256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="l"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109517056"/>
+        <c:crossAx val="83606528"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="109517056"/>
+        <c:axId val="83606528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1036,7 +1041,8 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="109515520"/>
+        <c:crossAx val="77584256"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
@@ -1044,7 +1050,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1199,11 +1205,11 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="100"/>
-        <c:axId val="132033920"/>
-        <c:axId val="132035712"/>
+        <c:axId val="93581696"/>
+        <c:axId val="93948544"/>
       </c:barChart>
       <c:valAx>
-        <c:axId val="132035712"/>
+        <c:axId val="93948544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1221,18 +1227,20 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="132033920"/>
+        <c:crossAx val="93581696"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="132033920"/>
+        <c:axId val="93581696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="l"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="132035712"/>
+        <c:crossAx val="93948544"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -1242,7 +1250,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1280,7 +1288,7 @@
                   </a:outerShdw>
                 </a:effectLst>
               </a:rPr>
-              <a:t>Top Ten File Types</a:t>
+              <a:t>Top Ten File Types By Count</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1353,36 +1361,36 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ChartData!$D$29:$D$37</c:f>
+              <c:f>ChartData!$C$29:$C$37</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>2364598238</c:v>
+                  <c:v>26723</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>35198654</c:v>
+                  <c:v>3512</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6515136</c:v>
+                  <c:v>3126</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1354416</c:v>
+                  <c:v>2364</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>285946541</c:v>
+                  <c:v>1025</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>641854581</c:v>
+                  <c:v>843</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>216855966</c:v>
+                  <c:v>398</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3241651</c:v>
+                  <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9565453</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1398,7 +1406,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1860,6 +1868,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -1876,10 +1885,10 @@
     <col min="1" max="1" width="21.7109375" customWidth="1"/>
     <col min="2" max="2" width="28" customWidth="1"/>
     <col min="3" max="3" width="14.85546875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.28515625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75">
@@ -1890,10 +1899,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>3</v>
@@ -1902,7 +1911,7 @@
         <v>226</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1915,8 +1924,8 @@
       <c r="C2" s="3">
         <v>90814</v>
       </c>
-      <c r="D2" s="6">
-        <f>C2/SUM(C$2:C$101)</f>
+      <c r="D2" s="5">
+        <f t="shared" ref="D2:D33" si="0">C2/SUM(C$2:C$101)</f>
         <v>3.289719869923953E-2</v>
       </c>
       <c r="E2" s="3">
@@ -1925,8 +1934,8 @@
       <c r="F2" s="3">
         <v>21244928</v>
       </c>
-      <c r="G2" s="6">
-        <f>F2/SUM(F$2:F$101)</f>
+      <c r="G2" s="5">
+        <f t="shared" ref="G2:G33" si="1">F2/SUM(F$2:F$101)</f>
         <v>7.7015651843371684E-3</v>
       </c>
     </row>
@@ -1940,8 +1949,8 @@
       <c r="C3" s="3">
         <v>89284</v>
       </c>
-      <c r="D3" s="6">
-        <f>C3/SUM(C$2:C$101)</f>
+      <c r="D3" s="5">
+        <f t="shared" si="0"/>
         <v>3.2342959110521534E-2</v>
       </c>
       <c r="E3" s="3">
@@ -1950,8 +1959,8 @@
       <c r="F3" s="3">
         <v>35939328</v>
       </c>
-      <c r="G3" s="6">
-        <f>F3/SUM(F$2:F$101)</f>
+      <c r="G3" s="5">
+        <f t="shared" si="1"/>
         <v>1.30284780100584E-2</v>
       </c>
     </row>
@@ -1965,8 +1974,8 @@
       <c r="C4" s="3">
         <v>80233</v>
       </c>
-      <c r="D4" s="6">
-        <f>C4/SUM(C$2:C$101)</f>
+      <c r="D4" s="5">
+        <f t="shared" si="0"/>
         <v>2.9064251582752498E-2</v>
       </c>
       <c r="E4" s="3">
@@ -1975,8 +1984,8 @@
       <c r="F4" s="3">
         <v>8943616</v>
       </c>
-      <c r="G4" s="6">
-        <f>F4/SUM(F$2:F$101)</f>
+      <c r="G4" s="5">
+        <f t="shared" si="1"/>
         <v>3.2421781616619673E-3</v>
       </c>
     </row>
@@ -1990,8 +1999,8 @@
       <c r="C5" s="3">
         <v>78333</v>
       </c>
-      <c r="D5" s="6">
-        <f>C5/SUM(C$2:C$101)</f>
+      <c r="D5" s="5">
+        <f t="shared" si="0"/>
         <v>2.8375980198070014E-2</v>
       </c>
       <c r="E5" s="3">
@@ -2000,8 +2009,8 @@
       <c r="F5" s="3">
         <v>439296</v>
       </c>
-      <c r="G5" s="6">
-        <f>F5/SUM(F$2:F$101)</f>
+      <c r="G5" s="5">
+        <f t="shared" si="1"/>
         <v>1.5925056461563817E-4</v>
       </c>
     </row>
@@ -2015,8 +2024,8 @@
       <c r="C6" s="3">
         <v>74316</v>
       </c>
-      <c r="D6" s="6">
-        <f>C6/SUM(C$2:C$101)</f>
+      <c r="D6" s="5">
+        <f t="shared" si="0"/>
         <v>2.6920829591612364E-2</v>
       </c>
       <c r="E6" s="3">
@@ -2025,8 +2034,8 @@
       <c r="F6" s="3">
         <v>13654016</v>
       </c>
-      <c r="G6" s="6">
-        <f>F6/SUM(F$2:F$101)</f>
+      <c r="G6" s="5">
+        <f t="shared" si="1"/>
         <v>4.949759973391421E-3</v>
       </c>
     </row>
@@ -2040,8 +2049,8 @@
       <c r="C7" s="3">
         <v>73410</v>
       </c>
-      <c r="D7" s="6">
-        <f>C7/SUM(C$2:C$101)</f>
+      <c r="D7" s="5">
+        <f t="shared" si="0"/>
         <v>2.6592632815547978E-2</v>
       </c>
       <c r="E7" s="3">
@@ -2050,8 +2059,8 @@
       <c r="F7" s="3">
         <v>27280384</v>
       </c>
-      <c r="G7" s="6">
-        <f>F7/SUM(F$2:F$101)</f>
+      <c r="G7" s="5">
+        <f t="shared" si="1"/>
         <v>9.8894971839748637E-3</v>
       </c>
     </row>
@@ -2065,8 +2074,8 @@
       <c r="C8" s="3">
         <v>71610</v>
       </c>
-      <c r="D8" s="6">
-        <f>C8/SUM(C$2:C$101)</f>
+      <c r="D8" s="5">
+        <f t="shared" si="0"/>
         <v>2.5940586240585626E-2</v>
       </c>
       <c r="E8" s="3">
@@ -2075,8 +2084,8 @@
       <c r="F8" s="3">
         <v>82173952</v>
       </c>
-      <c r="G8" s="6">
-        <f>F8/SUM(F$2:F$101)</f>
+      <c r="G8" s="5">
+        <f t="shared" si="1"/>
         <v>2.9789135919057651E-2</v>
       </c>
     </row>
@@ -2090,8 +2099,8 @@
       <c r="C9" s="3">
         <v>67431</v>
       </c>
-      <c r="D9" s="6">
-        <f>C9/SUM(C$2:C$101)</f>
+      <c r="D9" s="5">
+        <f t="shared" si="0"/>
         <v>2.4426751442381361E-2</v>
       </c>
       <c r="E9" s="3">
@@ -2100,8 +2109,8 @@
       <c r="F9" s="3">
         <v>19748864</v>
       </c>
-      <c r="G9" s="6">
-        <f>F9/SUM(F$2:F$101)</f>
+      <c r="G9" s="5">
+        <f t="shared" si="1"/>
         <v>7.1592223523944008E-3</v>
       </c>
     </row>
@@ -2115,8 +2124,8 @@
       <c r="C10" s="3">
         <v>66046</v>
       </c>
-      <c r="D10" s="6">
-        <f>C10/SUM(C$2:C$101)</f>
+      <c r="D10" s="5">
+        <f t="shared" si="0"/>
         <v>2.392503782775755E-2</v>
       </c>
       <c r="E10" s="3">
@@ -2125,8 +2134,8 @@
       <c r="F10" s="3">
         <v>47084544</v>
       </c>
-      <c r="G10" s="6">
-        <f>F10/SUM(F$2:F$101)</f>
+      <c r="G10" s="5">
+        <f t="shared" si="1"/>
         <v>1.7068765061985219E-2</v>
       </c>
     </row>
@@ -2140,8 +2149,8 @@
       <c r="C11" s="3">
         <v>65533</v>
       </c>
-      <c r="D11" s="6">
-        <f>C11/SUM(C$2:C$101)</f>
+      <c r="D11" s="5">
+        <f t="shared" si="0"/>
         <v>2.3739204553893278E-2</v>
       </c>
       <c r="E11" s="3">
@@ -2150,8 +2159,8 @@
       <c r="F11" s="3">
         <v>88934400</v>
       </c>
-      <c r="G11" s="6">
-        <f>F11/SUM(F$2:F$101)</f>
+      <c r="G11" s="5">
+        <f t="shared" si="1"/>
         <v>3.2239887032326754E-2</v>
       </c>
     </row>
@@ -2165,8 +2174,8 @@
       <c r="C12" s="3">
         <v>63248</v>
       </c>
-      <c r="D12" s="6">
-        <f>C12/SUM(C$2:C$101)</f>
+      <c r="D12" s="5">
+        <f t="shared" si="0"/>
         <v>2.2911467651788291E-2</v>
       </c>
       <c r="E12" s="3">
@@ -2175,8 +2184,8 @@
       <c r="F12" s="3">
         <v>4937728</v>
       </c>
-      <c r="G12" s="6">
-        <f>F12/SUM(F$2:F$101)</f>
+      <c r="G12" s="5">
+        <f t="shared" si="1"/>
         <v>1.7899911948172664E-3</v>
       </c>
     </row>
@@ -2190,8 +2199,8 @@
       <c r="C13" s="3">
         <v>63053</v>
       </c>
-      <c r="D13" s="6">
-        <f>C13/SUM(C$2:C$101)</f>
+      <c r="D13" s="5">
+        <f t="shared" si="0"/>
         <v>2.2840829272834037E-2</v>
       </c>
       <c r="E13" s="3">
@@ -2200,8 +2209,8 @@
       <c r="F13" s="3">
         <v>4466688</v>
       </c>
-      <c r="G13" s="6">
-        <f>F13/SUM(F$2:F$101)</f>
+      <c r="G13" s="5">
+        <f t="shared" si="1"/>
         <v>1.619233013644321E-3</v>
       </c>
     </row>
@@ -2215,8 +2224,8 @@
       <c r="C14" s="3">
         <v>62581</v>
       </c>
-      <c r="D14" s="6">
-        <f>C14/SUM(C$2:C$101)</f>
+      <c r="D14" s="5">
+        <f t="shared" si="0"/>
         <v>2.266984817095502E-2</v>
       </c>
       <c r="E14" s="3">
@@ -2225,8 +2234,8 @@
       <c r="F14" s="3">
         <v>4065280</v>
       </c>
-      <c r="G14" s="6">
-        <f>F14/SUM(F$2:F$101)</f>
+      <c r="G14" s="5">
+        <f t="shared" si="1"/>
         <v>1.473717346209985E-3</v>
       </c>
     </row>
@@ -2240,8 +2249,8 @@
       <c r="C15" s="3">
         <v>62034</v>
       </c>
-      <c r="D15" s="6">
-        <f>C15/SUM(C$2:C$101)</f>
+      <c r="D15" s="5">
+        <f t="shared" si="0"/>
         <v>2.2471698461785906E-2</v>
       </c>
       <c r="E15" s="3">
@@ -2250,8 +2259,8 @@
       <c r="F15" s="3">
         <v>11546624</v>
       </c>
-      <c r="G15" s="6">
-        <f>F15/SUM(F$2:F$101)</f>
+      <c r="G15" s="5">
+        <f t="shared" si="1"/>
         <v>4.1858027193611563E-3</v>
       </c>
     </row>
@@ -2265,8 +2274,8 @@
       <c r="C16" s="3">
         <v>61313</v>
       </c>
-      <c r="D16" s="6">
-        <f>C16/SUM(C$2:C$101)</f>
+      <c r="D16" s="5">
+        <f t="shared" si="0"/>
         <v>2.2210517583703761E-2</v>
       </c>
       <c r="E16" s="3">
@@ -2275,8 +2284,8 @@
       <c r="F16" s="3">
         <v>120832</v>
       </c>
-      <c r="G16" s="6">
-        <f>F16/SUM(F$2:F$101)</f>
+      <c r="G16" s="5">
+        <f t="shared" si="1"/>
         <v>4.3803185605233813E-5</v>
       </c>
     </row>
@@ -2290,8 +2299,8 @@
       <c r="C17" s="3">
         <v>59574</v>
       </c>
-      <c r="D17" s="6">
-        <f>C17/SUM(C$2:C$101)</f>
+      <c r="D17" s="5">
+        <f t="shared" si="0"/>
         <v>2.1580568142670689E-2</v>
       </c>
       <c r="E17" s="3">
@@ -2300,8 +2309,8 @@
       <c r="F17" s="3">
         <v>26083328</v>
       </c>
-      <c r="G17" s="6">
-        <f>F17/SUM(F$2:F$101)</f>
+      <c r="G17" s="5">
+        <f t="shared" si="1"/>
         <v>9.4555486757331841E-3</v>
       </c>
     </row>
@@ -2315,8 +2324,8 @@
       <c r="C18" s="3">
         <v>55394</v>
       </c>
-      <c r="D18" s="6">
-        <f>C18/SUM(C$2:C$101)</f>
+      <c r="D18" s="5">
+        <f t="shared" si="0"/>
         <v>2.0066371096369225E-2</v>
       </c>
       <c r="E18" s="3">
@@ -2325,8 +2334,8 @@
       <c r="F18" s="3">
         <v>21957632</v>
       </c>
-      <c r="G18" s="6">
-        <f>F18/SUM(F$2:F$101)</f>
+      <c r="G18" s="5">
+        <f t="shared" si="1"/>
         <v>7.9599297367205814E-3</v>
       </c>
     </row>
@@ -2340,8 +2349,8 @@
       <c r="C19" s="3">
         <v>55219</v>
       </c>
-      <c r="D19" s="6">
-        <f>C19/SUM(C$2:C$101)</f>
+      <c r="D19" s="5">
+        <f t="shared" si="0"/>
         <v>2.0002977679358994E-2</v>
       </c>
       <c r="E19" s="3">
@@ -2350,8 +2359,8 @@
       <c r="F19" s="3">
         <v>96608256</v>
       </c>
-      <c r="G19" s="6">
-        <f>F19/SUM(F$2:F$101)</f>
+      <c r="G19" s="5">
+        <f t="shared" si="1"/>
         <v>3.5021760531696429E-2</v>
       </c>
     </row>
@@ -2365,8 +2374,8 @@
       <c r="C20" s="3">
         <v>54124</v>
       </c>
-      <c r="D20" s="6">
-        <f>C20/SUM(C$2:C$101)</f>
+      <c r="D20" s="5">
+        <f t="shared" si="0"/>
         <v>1.9606316012923564E-2</v>
       </c>
       <c r="E20" s="3">
@@ -2375,8 +2384,8 @@
       <c r="F20" s="3">
         <v>12575744</v>
       </c>
-      <c r="G20" s="6">
-        <f>F20/SUM(F$2:F$101)</f>
+      <c r="G20" s="5">
+        <f t="shared" si="1"/>
         <v>4.5588722238803087E-3</v>
       </c>
     </row>
@@ -2390,8 +2399,8 @@
       <c r="C21" s="3">
         <v>53448</v>
       </c>
-      <c r="D21" s="6">
-        <f>C21/SUM(C$2:C$101)</f>
+      <c r="D21" s="5">
+        <f t="shared" si="0"/>
         <v>1.9361436299215478E-2</v>
       </c>
       <c r="E21" s="3">
@@ -2400,8 +2409,8 @@
       <c r="F21" s="3">
         <v>31313920</v>
       </c>
-      <c r="G21" s="6">
-        <f>F21/SUM(F$2:F$101)</f>
+      <c r="G21" s="5">
+        <f t="shared" si="1"/>
         <v>1.1351706913627543E-2</v>
       </c>
     </row>
@@ -2415,8 +2424,8 @@
       <c r="C22" s="3">
         <v>52502</v>
       </c>
-      <c r="D22" s="6">
-        <f>C22/SUM(C$2:C$101)</f>
+      <c r="D22" s="5">
+        <f t="shared" si="0"/>
         <v>1.9018749599263043E-2</v>
       </c>
       <c r="E22" s="3">
@@ -2425,8 +2434,8 @@
       <c r="F22" s="3">
         <v>32891904</v>
       </c>
-      <c r="G22" s="6">
-        <f>F22/SUM(F$2:F$101)</f>
+      <c r="G22" s="5">
+        <f t="shared" si="1"/>
         <v>1.192374682055691E-2</v>
       </c>
     </row>
@@ -2440,8 +2449,8 @@
       <c r="C23" s="3">
         <v>49187</v>
       </c>
-      <c r="D23" s="6">
-        <f>C23/SUM(C$2:C$101)</f>
+      <c r="D23" s="5">
+        <f t="shared" si="0"/>
         <v>1.781789715704071E-2</v>
       </c>
       <c r="E23" s="3">
@@ -2450,8 +2459,8 @@
       <c r="F23" s="3">
         <v>61043712</v>
       </c>
-      <c r="G23" s="6">
-        <f>F23/SUM(F$2:F$101)</f>
+      <c r="G23" s="5">
+        <f t="shared" si="1"/>
         <v>2.2129146639701721E-2</v>
       </c>
     </row>
@@ -2465,8 +2474,8 @@
       <c r="C24" s="3">
         <v>48564</v>
       </c>
-      <c r="D24" s="6">
-        <f>C24/SUM(C$2:C$101)</f>
+      <c r="D24" s="5">
+        <f t="shared" si="0"/>
         <v>1.7592216592484295E-2</v>
       </c>
       <c r="E24" s="3">
@@ -2475,8 +2484,8 @@
       <c r="F24" s="3">
         <v>27423744</v>
       </c>
-      <c r="G24" s="6">
-        <f>F24/SUM(F$2:F$101)</f>
+      <c r="G24" s="5">
+        <f t="shared" si="1"/>
         <v>9.9414670652014127E-3</v>
       </c>
     </row>
@@ -2490,8 +2499,8 @@
       <c r="C25" s="3">
         <v>46111</v>
       </c>
-      <c r="D25" s="6">
-        <f>C25/SUM(C$2:C$101)</f>
+      <c r="D25" s="5">
+        <f t="shared" si="0"/>
         <v>1.6703622010049487E-2</v>
       </c>
       <c r="E25" s="3">
@@ -2500,8 +2509,8 @@
       <c r="F25" s="3">
         <v>30368768</v>
       </c>
-      <c r="G25" s="6">
-        <f>F25/SUM(F$2:F$101)</f>
+      <c r="G25" s="5">
+        <f t="shared" si="1"/>
         <v>1.1009076910969653E-2</v>
       </c>
     </row>
@@ -2515,8 +2524,8 @@
       <c r="C26" s="3">
         <v>44457</v>
       </c>
-      <c r="D26" s="6">
-        <f>C26/SUM(C$2:C$101)</f>
+      <c r="D26" s="5">
+        <f t="shared" si="0"/>
         <v>1.6104463657278523E-2</v>
       </c>
       <c r="E26" s="3">
@@ -2525,8 +2534,8 @@
       <c r="F26" s="3">
         <v>58786816</v>
       </c>
-      <c r="G26" s="6">
-        <f>F26/SUM(F$2:F$101)</f>
+      <c r="G26" s="5">
+        <f t="shared" si="1"/>
         <v>2.1310992223820914E-2</v>
       </c>
     </row>
@@ -2540,8 +2549,8 @@
       <c r="C27" s="3">
         <v>44306</v>
       </c>
-      <c r="D27" s="6">
-        <f>C27/SUM(C$2:C$101)</f>
+      <c r="D27" s="5">
+        <f t="shared" si="0"/>
         <v>1.6049764194601128E-2</v>
       </c>
       <c r="E27" s="3">
@@ -2550,8 +2559,8 @@
       <c r="F27" s="3">
         <v>11675648</v>
       </c>
-      <c r="G27" s="6">
-        <f>F27/SUM(F$2:F$101)</f>
+      <c r="G27" s="5">
+        <f t="shared" si="1"/>
         <v>4.2325756124650506E-3</v>
       </c>
     </row>
@@ -2565,8 +2574,8 @@
       <c r="C28" s="3">
         <v>42935</v>
       </c>
-      <c r="D28" s="6">
-        <f>C28/SUM(C$2:C$101)</f>
+      <c r="D28" s="5">
+        <f t="shared" si="0"/>
         <v>1.5553122053338135E-2</v>
       </c>
       <c r="E28" s="3">
@@ -2575,8 +2584,8 @@
       <c r="F28" s="3">
         <v>5321728</v>
       </c>
-      <c r="G28" s="6">
-        <f>F28/SUM(F$2:F$101)</f>
+      <c r="G28" s="5">
+        <f t="shared" si="1"/>
         <v>1.9291962338169502E-3</v>
       </c>
     </row>
@@ -2590,8 +2599,8 @@
       <c r="C29" s="3">
         <v>41953</v>
       </c>
-      <c r="D29" s="6">
-        <f>C29/SUM(C$2:C$101)</f>
+      <c r="D29" s="5">
+        <f t="shared" si="0"/>
         <v>1.5197394421886451E-2</v>
       </c>
       <c r="E29" s="3">
@@ -2600,8 +2609,8 @@
       <c r="F29" s="3">
         <v>9598976</v>
       </c>
-      <c r="G29" s="6">
-        <f>F29/SUM(F$2:F$101)</f>
+      <c r="G29" s="5">
+        <f t="shared" si="1"/>
         <v>3.4797547615547605E-3</v>
       </c>
     </row>
@@ -2615,8 +2624,8 @@
       <c r="C30" s="3">
         <v>38800</v>
       </c>
-      <c r="D30" s="6">
-        <f>C30/SUM(C$2:C$101)</f>
+      <c r="D30" s="5">
+        <f t="shared" si="0"/>
         <v>1.4055226171410728E-2</v>
       </c>
       <c r="E30" s="3">
@@ -2625,8 +2634,8 @@
       <c r="F30" s="3">
         <v>2423808</v>
       </c>
-      <c r="G30" s="6">
-        <f>F30/SUM(F$2:F$101)</f>
+      <c r="G30" s="5">
+        <f t="shared" si="1"/>
         <v>8.7866220616600365E-4</v>
       </c>
     </row>
@@ -2640,8 +2649,8 @@
       <c r="C31" s="3">
         <v>37944</v>
       </c>
-      <c r="D31" s="6">
-        <f>C31/SUM(C$2:C$101)</f>
+      <c r="D31" s="5">
+        <f t="shared" si="0"/>
         <v>1.3745141800206409E-2</v>
       </c>
       <c r="E31" s="3">
@@ -2650,8 +2659,8 @@
       <c r="F31" s="3">
         <v>34450432</v>
       </c>
-      <c r="G31" s="6">
-        <f>F31/SUM(F$2:F$101)</f>
+      <c r="G31" s="5">
+        <f t="shared" si="1"/>
         <v>1.2488733672176958E-2</v>
       </c>
     </row>
@@ -2665,8 +2674,8 @@
       <c r="C32" s="3">
         <v>37265</v>
       </c>
-      <c r="D32" s="6">
-        <f>C32/SUM(C$2:C$101)</f>
+      <c r="D32" s="5">
+        <f t="shared" si="0"/>
         <v>1.3499175342206722E-2</v>
       </c>
       <c r="E32" s="3">
@@ -2675,8 +2684,8 @@
       <c r="F32" s="3">
         <v>8229888</v>
       </c>
-      <c r="G32" s="6">
-        <f>F32/SUM(F$2:F$101)</f>
+      <c r="G32" s="5">
+        <f t="shared" si="1"/>
         <v>2.9834423958412216E-3</v>
       </c>
     </row>
@@ -2690,8 +2699,8 @@
       <c r="C33" s="3">
         <v>36748</v>
       </c>
-      <c r="D33" s="6">
-        <f>C33/SUM(C$2:C$101)</f>
+      <c r="D33" s="5">
+        <f t="shared" si="0"/>
         <v>1.3311893075953646E-2</v>
       </c>
       <c r="E33" s="3">
@@ -2700,8 +2709,8 @@
       <c r="F33" s="3">
         <v>54841344</v>
       </c>
-      <c r="G33" s="6">
-        <f>F33/SUM(F$2:F$101)</f>
+      <c r="G33" s="5">
+        <f t="shared" si="1"/>
         <v>1.9880706849778832E-2</v>
       </c>
     </row>
@@ -2715,8 +2724,8 @@
       <c r="C34" s="3">
         <v>33092</v>
       </c>
-      <c r="D34" s="6">
-        <f>C34/SUM(C$2:C$101)</f>
+      <c r="D34" s="5">
+        <f t="shared" ref="D34:D65" si="2">C34/SUM(C$2:C$101)</f>
         <v>1.1987514032585665E-2</v>
       </c>
       <c r="E34" s="3">
@@ -2725,8 +2734,8 @@
       <c r="F34" s="3">
         <v>13153280</v>
       </c>
-      <c r="G34" s="6">
-        <f>F34/SUM(F$2:F$101)</f>
+      <c r="G34" s="5">
+        <f t="shared" ref="G34:G65" si="3">F34/SUM(F$2:F$101)</f>
         <v>4.7682366025358332E-3</v>
       </c>
     </row>
@@ -2740,8 +2749,8 @@
       <c r="C35" s="3">
         <v>33006</v>
       </c>
-      <c r="D35" s="6">
-        <f>C35/SUM(C$2:C$101)</f>
+      <c r="D35" s="5">
+        <f t="shared" si="2"/>
         <v>1.1956360696226354E-2</v>
       </c>
       <c r="E35" s="3">
@@ -2750,8 +2759,8 @@
       <c r="F35" s="3">
         <v>45662208</v>
       </c>
-      <c r="G35" s="6">
-        <f>F35/SUM(F$2:F$101)</f>
+      <c r="G35" s="5">
+        <f t="shared" si="3"/>
         <v>1.6553149597530393E-2</v>
       </c>
     </row>
@@ -2765,8 +2774,8 @@
       <c r="C36" s="3">
         <v>32953</v>
       </c>
-      <c r="D36" s="6">
-        <f>C36/SUM(C$2:C$101)</f>
+      <c r="D36" s="5">
+        <f t="shared" si="2"/>
         <v>1.1937161547074684E-2</v>
       </c>
       <c r="E36" s="3">
@@ -2775,8 +2784,8 @@
       <c r="F36" s="3">
         <v>1338368</v>
       </c>
-      <c r="G36" s="6">
-        <f>F36/SUM(F$2:F$101)</f>
+      <c r="G36" s="5">
+        <f t="shared" si="3"/>
         <v>4.8517596259356434E-4</v>
       </c>
     </row>
@@ -2790,8 +2799,8 @@
       <c r="C37" s="3">
         <v>32126</v>
       </c>
-      <c r="D37" s="6">
-        <f>C37/SUM(C$2:C$101)</f>
+      <c r="D37" s="5">
+        <f t="shared" si="2"/>
         <v>1.1637582370689202E-2</v>
       </c>
       <c r="E37" s="3">
@@ -2800,8 +2809,8 @@
       <c r="F37" s="3">
         <v>35878912</v>
       </c>
-      <c r="G37" s="6">
-        <f>F37/SUM(F$2:F$101)</f>
+      <c r="G37" s="5">
+        <f t="shared" si="3"/>
         <v>1.3006576417255783E-2</v>
       </c>
     </row>
@@ -2815,8 +2824,8 @@
       <c r="C38" s="3">
         <v>30072</v>
       </c>
-      <c r="D38" s="6">
-        <f>C38/SUM(C$2:C$101)</f>
+      <c r="D38" s="5">
+        <f t="shared" si="2"/>
         <v>1.0893524779037716E-2</v>
       </c>
       <c r="E38" s="3">
@@ -2825,8 +2834,8 @@
       <c r="F38" s="3">
         <v>32401408</v>
       </c>
-      <c r="G38" s="6">
-        <f>F38/SUM(F$2:F$101)</f>
+      <c r="G38" s="5">
+        <f t="shared" si="3"/>
         <v>1.1745935584074647E-2</v>
       </c>
     </row>
@@ -2840,8 +2849,8 @@
       <c r="C39" s="3">
         <v>29779</v>
       </c>
-      <c r="D39" s="6">
-        <f>C39/SUM(C$2:C$101)</f>
+      <c r="D39" s="5">
+        <f t="shared" si="2"/>
         <v>1.0787386086557734E-2</v>
       </c>
       <c r="E39" s="3">
@@ -2850,8 +2859,8 @@
       <c r="F39" s="3">
         <v>20370432</v>
       </c>
-      <c r="G39" s="6">
-        <f>F39/SUM(F$2:F$101)</f>
+      <c r="G39" s="5">
+        <f t="shared" si="3"/>
         <v>7.3845489088552223E-3</v>
       </c>
     </row>
@@ -2865,8 +2874,8 @@
       <c r="C40" s="3">
         <v>29628</v>
       </c>
-      <c r="D40" s="6">
-        <f>C40/SUM(C$2:C$101)</f>
+      <c r="D40" s="5">
+        <f t="shared" si="2"/>
         <v>1.0732686623880336E-2</v>
       </c>
       <c r="E40" s="3">
@@ -2875,8 +2884,8 @@
       <c r="F40" s="3">
         <v>31490048</v>
       </c>
-      <c r="G40" s="6">
-        <f>F40/SUM(F$2:F$101)</f>
+      <c r="G40" s="5">
+        <f t="shared" si="3"/>
         <v>1.1415555624848731E-2</v>
       </c>
     </row>
@@ -2890,8 +2899,8 @@
       <c r="C41" s="3">
         <v>29256</v>
       </c>
-      <c r="D41" s="6">
-        <f>C41/SUM(C$2:C$101)</f>
+      <c r="D41" s="5">
+        <f t="shared" si="2"/>
         <v>1.0597930331721451E-2</v>
       </c>
       <c r="E41" s="3">
@@ -2900,8 +2909,8 @@
       <c r="F41" s="3">
         <v>39303168</v>
       </c>
-      <c r="G41" s="6">
-        <f>F41/SUM(F$2:F$101)</f>
+      <c r="G41" s="5">
+        <f t="shared" si="3"/>
         <v>1.4247914151695629E-2</v>
       </c>
     </row>
@@ -2915,8 +2924,8 @@
       <c r="C42" s="3">
         <v>28174</v>
       </c>
-      <c r="D42" s="6">
-        <f>C42/SUM(C$2:C$101)</f>
+      <c r="D42" s="5">
+        <f t="shared" si="2"/>
         <v>1.0205977890549636E-2</v>
       </c>
       <c r="E42" s="3">
@@ -2925,8 +2934,8 @@
       <c r="F42" s="3">
         <v>8918016</v>
       </c>
-      <c r="G42" s="6">
-        <f>F42/SUM(F$2:F$101)</f>
+      <c r="G42" s="5">
+        <f t="shared" si="3"/>
         <v>3.2328978257286549E-3</v>
       </c>
     </row>
@@ -2940,8 +2949,8 @@
       <c r="C43" s="3">
         <v>26663</v>
       </c>
-      <c r="D43" s="6">
-        <f>C43/SUM(C$2:C$101)</f>
+      <c r="D43" s="5">
+        <f t="shared" si="2"/>
         <v>9.6586210156784594E-3</v>
       </c>
       <c r="E43" s="3">
@@ -2950,8 +2959,8 @@
       <c r="F43" s="3">
         <v>12265472</v>
       </c>
-      <c r="G43" s="6">
-        <f>F43/SUM(F$2:F$101)</f>
+      <c r="G43" s="5">
+        <f t="shared" si="3"/>
         <v>4.4463945523685643E-3</v>
       </c>
     </row>
@@ -2965,8 +2974,8 @@
       <c r="C44" s="3">
         <v>25411</v>
       </c>
-      <c r="D44" s="6">
-        <f>C44/SUM(C$2:C$101)</f>
+      <c r="D44" s="5">
+        <f t="shared" si="2"/>
         <v>9.2050863979824225E-3</v>
       </c>
       <c r="E44" s="3">
@@ -2975,8 +2984,8 @@
       <c r="F44" s="3">
         <v>35002368</v>
       </c>
-      <c r="G44" s="6">
-        <f>F44/SUM(F$2:F$101)</f>
+      <c r="G44" s="5">
+        <f t="shared" si="3"/>
         <v>1.2688817714899171E-2</v>
       </c>
     </row>
@@ -2990,8 +2999,8 @@
       <c r="C45" s="3">
         <v>24994</v>
       </c>
-      <c r="D45" s="6">
-        <f>C45/SUM(C$2:C$101)</f>
+      <c r="D45" s="5">
+        <f t="shared" si="2"/>
         <v>9.0540289414494778E-3</v>
       </c>
       <c r="E45" s="3">
@@ -3000,8 +3009,8 @@
       <c r="F45" s="3">
         <v>13421568</v>
       </c>
-      <c r="G45" s="6">
-        <f>F45/SUM(F$2:F$101)</f>
+      <c r="G45" s="5">
+        <f t="shared" si="3"/>
         <v>4.8654945231169453E-3</v>
       </c>
     </row>
@@ -3015,8 +3024,8 @@
       <c r="C46" s="3">
         <v>24312</v>
       </c>
-      <c r="D46" s="6">
-        <f>C46/SUM(C$2:C$101)</f>
+      <c r="D46" s="5">
+        <f t="shared" si="2"/>
         <v>8.8069757391581859E-3</v>
       </c>
       <c r="E46" s="3">
@@ -3025,8 +3034,8 @@
       <c r="F46" s="3">
         <v>17687552</v>
       </c>
-      <c r="G46" s="6">
-        <f>F46/SUM(F$2:F$101)</f>
+      <c r="G46" s="5">
+        <f t="shared" si="3"/>
         <v>6.4119697030440986E-3</v>
       </c>
     </row>
@@ -3040,8 +3049,8 @@
       <c r="C47" s="3">
         <v>24120</v>
       </c>
-      <c r="D47" s="6">
-        <f>C47/SUM(C$2:C$101)</f>
+      <c r="D47" s="5">
+        <f t="shared" si="2"/>
         <v>8.7374241044955343E-3</v>
       </c>
       <c r="E47" s="3">
@@ -3050,8 +3059,8 @@
       <c r="F47" s="3">
         <v>14260224</v>
       </c>
-      <c r="G47" s="6">
-        <f>F47/SUM(F$2:F$101)</f>
+      <c r="G47" s="5">
+        <f t="shared" si="3"/>
         <v>5.169518328292255E-3</v>
       </c>
     </row>
@@ -3065,8 +3074,8 @@
       <c r="C48" s="3">
         <v>24073</v>
       </c>
-      <c r="D48" s="6">
-        <f>C48/SUM(C$2:C$101)</f>
+      <c r="D48" s="5">
+        <f t="shared" si="2"/>
         <v>8.7203984439270729E-3</v>
       </c>
       <c r="E48" s="3">
@@ -3075,8 +3084,8 @@
       <c r="F48" s="3">
         <v>41385984</v>
       </c>
-      <c r="G48" s="6">
-        <f>F48/SUM(F$2:F$101)</f>
+      <c r="G48" s="5">
+        <f t="shared" si="3"/>
         <v>1.5002962283229913E-2</v>
       </c>
     </row>
@@ -3090,8 +3099,8 @@
       <c r="C49" s="3">
         <v>23903</v>
       </c>
-      <c r="D49" s="6">
-        <f>C49/SUM(C$2:C$101)</f>
+      <c r="D49" s="5">
+        <f t="shared" si="2"/>
         <v>8.6588162674028513E-3</v>
       </c>
       <c r="E49" s="3">
@@ -3100,8 +3109,8 @@
       <c r="F49" s="3">
         <v>7200768</v>
       </c>
-      <c r="G49" s="6">
-        <f>F49/SUM(F$2:F$101)</f>
+      <c r="G49" s="5">
+        <f t="shared" si="3"/>
         <v>2.6103728913220692E-3</v>
       </c>
     </row>
@@ -3115,8 +3124,8 @@
       <c r="C50" s="3">
         <v>22688</v>
       </c>
-      <c r="D50" s="6">
-        <f>C50/SUM(C$2:C$101)</f>
+      <c r="D50" s="5">
+        <f t="shared" si="2"/>
         <v>8.2186848293032636E-3</v>
       </c>
       <c r="E50" s="3">
@@ -3125,8 +3134,8 @@
       <c r="F50" s="3">
         <v>48828416</v>
       </c>
-      <c r="G50" s="6">
-        <f>F50/SUM(F$2:F$101)</f>
+      <c r="G50" s="5">
+        <f t="shared" si="3"/>
         <v>1.770094154576245E-2</v>
       </c>
     </row>
@@ -3140,8 +3149,8 @@
       <c r="C51" s="3">
         <v>22524</v>
       </c>
-      <c r="D51" s="6">
-        <f>C51/SUM(C$2:C$101)</f>
+      <c r="D51" s="5">
+        <f t="shared" si="2"/>
         <v>8.1592761413622483E-3</v>
       </c>
       <c r="E51" s="3">
@@ -3150,8 +3159,8 @@
       <c r="F51" s="3">
         <v>20372480</v>
       </c>
-      <c r="G51" s="6">
-        <f>F51/SUM(F$2:F$101)</f>
+      <c r="G51" s="5">
+        <f t="shared" si="3"/>
         <v>7.385291335729887E-3</v>
       </c>
     </row>
@@ -3165,8 +3174,8 @@
       <c r="C52" s="3">
         <v>22275</v>
       </c>
-      <c r="D52" s="6">
-        <f>C52/SUM(C$2:C$101)</f>
+      <c r="D52" s="5">
+        <f t="shared" si="2"/>
         <v>8.0690763651591231E-3</v>
       </c>
       <c r="E52" s="3">
@@ -3175,8 +3184,8 @@
       <c r="F52" s="3">
         <v>15578112</v>
       </c>
-      <c r="G52" s="6">
-        <f>F52/SUM(F$2:F$101)</f>
+      <c r="G52" s="5">
+        <f t="shared" si="3"/>
         <v>5.6472700221391692E-3</v>
       </c>
     </row>
@@ -3190,8 +3199,8 @@
       <c r="C53" s="3">
         <v>22251</v>
       </c>
-      <c r="D53" s="6">
-        <f>C53/SUM(C$2:C$101)</f>
+      <c r="D53" s="5">
+        <f t="shared" si="2"/>
         <v>8.060382410826291E-3</v>
       </c>
       <c r="E53" s="3">
@@ -3200,8 +3209,8 @@
       <c r="F53" s="3">
         <v>58795008</v>
       </c>
-      <c r="G53" s="6">
-        <f>F53/SUM(F$2:F$101)</f>
+      <c r="G53" s="5">
+        <f t="shared" si="3"/>
         <v>2.1313961931319576E-2</v>
       </c>
     </row>
@@ -3215,8 +3224,8 @@
       <c r="C54" s="3">
         <v>20894</v>
       </c>
-      <c r="D54" s="6">
-        <f>C54/SUM(C$2:C$101)</f>
+      <c r="D54" s="5">
+        <f t="shared" si="2"/>
         <v>7.5688117429241171E-3</v>
       </c>
       <c r="E54" s="3">
@@ -3225,8 +3234,8 @@
       <c r="F54" s="3">
         <v>1352704</v>
       </c>
-      <c r="G54" s="6">
-        <f>F54/SUM(F$2:F$101)</f>
+      <c r="G54" s="5">
+        <f t="shared" si="3"/>
         <v>4.9037295071621917E-4</v>
       </c>
     </row>
@@ -3240,8 +3249,8 @@
       <c r="C55" s="3">
         <v>19813</v>
       </c>
-      <c r="D55" s="6">
-        <f>C55/SUM(C$2:C$101)</f>
+      <c r="D55" s="5">
+        <f t="shared" si="2"/>
         <v>7.1772215498495037E-3</v>
       </c>
       <c r="E55" s="3">
@@ -3250,8 +3259,8 @@
       <c r="F55" s="3">
         <v>44510208</v>
       </c>
-      <c r="G55" s="6">
-        <f>F55/SUM(F$2:F$101)</f>
+      <c r="G55" s="5">
+        <f t="shared" si="3"/>
         <v>1.613553448053134E-2</v>
       </c>
     </row>
@@ -3265,8 +3274,8 @@
       <c r="C56" s="3">
         <v>19415</v>
       </c>
-      <c r="D56" s="6">
-        <f>C56/SUM(C$2:C$101)</f>
+      <c r="D56" s="5">
+        <f t="shared" si="2"/>
         <v>7.0330468071633833E-3</v>
       </c>
       <c r="E56" s="3">
@@ -3275,8 +3284,8 @@
       <c r="F56" s="3">
         <v>21013504</v>
       </c>
-      <c r="G56" s="6">
-        <f>F56/SUM(F$2:F$101)</f>
+      <c r="G56" s="5">
+        <f t="shared" si="3"/>
         <v>7.6176709475000264E-3</v>
       </c>
     </row>
@@ -3290,8 +3299,8 @@
       <c r="C57" s="3">
         <v>16861</v>
       </c>
-      <c r="D57" s="6">
-        <f>C57/SUM(C$2:C$101)</f>
+      <c r="D57" s="5">
+        <f t="shared" si="2"/>
         <v>6.1078651669112449E-3</v>
       </c>
       <c r="E57" s="3">
@@ -3300,8 +3309,8 @@
       <c r="F57" s="3">
         <v>27632640</v>
       </c>
-      <c r="G57" s="6">
-        <f>F57/SUM(F$2:F$101)</f>
+      <c r="G57" s="5">
+        <f t="shared" si="3"/>
         <v>1.0017194606417241E-2</v>
       </c>
     </row>
@@ -3315,8 +3324,8 @@
       <c r="C58" s="3">
         <v>16617</v>
       </c>
-      <c r="D58" s="6">
-        <f>C58/SUM(C$2:C$101)</f>
+      <c r="D58" s="5">
+        <f t="shared" si="2"/>
         <v>6.0194766311941258E-3</v>
       </c>
       <c r="E58" s="3">
@@ -3325,8 +3334,8 @@
       <c r="F58" s="3">
         <v>59581440</v>
       </c>
-      <c r="G58" s="6">
-        <f>F58/SUM(F$2:F$101)</f>
+      <c r="G58" s="5">
+        <f t="shared" si="3"/>
         <v>2.1599053851190927E-2</v>
       </c>
     </row>
@@ -3340,8 +3349,8 @@
       <c r="C59" s="3">
         <v>15088</v>
       </c>
-      <c r="D59" s="6">
-        <f>C59/SUM(C$2:C$101)</f>
+      <c r="D59" s="5">
+        <f t="shared" si="2"/>
         <v>5.4655992905733265E-3</v>
       </c>
       <c r="E59" s="3">
@@ -3350,8 +3359,8 @@
       <c r="F59" s="3">
         <v>4019200</v>
       </c>
-      <c r="G59" s="6">
-        <f>F59/SUM(F$2:F$101)</f>
+      <c r="G59" s="5">
+        <f t="shared" si="3"/>
         <v>1.4570127415300231E-3</v>
       </c>
     </row>
@@ -3365,8 +3374,8 @@
       <c r="C60" s="3">
         <v>14303</v>
       </c>
-      <c r="D60" s="6">
-        <f>C60/SUM(C$2:C$101)</f>
+      <c r="D60" s="5">
+        <f t="shared" si="2"/>
         <v>5.1812345342702997E-3</v>
       </c>
       <c r="E60" s="3">
@@ -3375,8 +3384,8 @@
       <c r="F60" s="3">
         <v>66073600</v>
       </c>
-      <c r="G60" s="6">
-        <f>F60/SUM(F$2:F$101)</f>
+      <c r="G60" s="5">
+        <f t="shared" si="3"/>
         <v>2.3952547043878912E-2</v>
       </c>
     </row>
@@ -3390,8 +3399,8 @@
       <c r="C61" s="3">
         <v>11837</v>
       </c>
-      <c r="D61" s="6">
-        <f>C61/SUM(C$2:C$101)</f>
+      <c r="D61" s="5">
+        <f t="shared" si="2"/>
         <v>4.2879307265718761E-3</v>
       </c>
       <c r="E61" s="3">
@@ -3400,8 +3409,8 @@
       <c r="F61" s="3">
         <v>27322368</v>
       </c>
-      <c r="G61" s="6">
-        <f>F61/SUM(F$2:F$101)</f>
+      <c r="G61" s="5">
+        <f t="shared" si="3"/>
         <v>9.9047169349054959E-3</v>
       </c>
     </row>
@@ -3415,8 +3424,8 @@
       <c r="C62" s="3">
         <v>11187</v>
       </c>
-      <c r="D62" s="6">
-        <f>C62/SUM(C$2:C$101)</f>
+      <c r="D62" s="5">
+        <f t="shared" si="2"/>
         <v>4.0524694633910265E-3</v>
       </c>
       <c r="E62" s="3">
@@ -3425,8 +3434,8 @@
       <c r="F62" s="3">
         <v>13082624</v>
       </c>
-      <c r="G62" s="6">
-        <f>F62/SUM(F$2:F$101)</f>
+      <c r="G62" s="5">
+        <f t="shared" si="3"/>
         <v>4.7426228753598915E-3</v>
       </c>
     </row>
@@ -3440,8 +3449,8 @@
       <c r="C63" s="3">
         <v>11044</v>
       </c>
-      <c r="D63" s="6">
-        <f>C63/SUM(C$2:C$101)</f>
+      <c r="D63" s="5">
+        <f t="shared" si="2"/>
         <v>4.0006679854912392E-3</v>
       </c>
       <c r="E63" s="3">
@@ -3450,8 +3459,8 @@
       <c r="F63" s="3">
         <v>47323136</v>
       </c>
-      <c r="G63" s="6">
-        <f>F63/SUM(F$2:F$101)</f>
+      <c r="G63" s="5">
+        <f t="shared" si="3"/>
         <v>1.7155257792883689E-2</v>
       </c>
     </row>
@@ -3465,8 +3474,8 @@
       <c r="C64" s="3">
         <v>10794</v>
       </c>
-      <c r="D64" s="6">
-        <f>C64/SUM(C$2:C$101)</f>
+      <c r="D64" s="5">
+        <f t="shared" si="2"/>
         <v>3.9101059611909121E-3</v>
       </c>
       <c r="E64" s="3">
@@ -3475,8 +3484,8 @@
       <c r="F64" s="3">
         <v>37381120</v>
       </c>
-      <c r="G64" s="6">
-        <f>F64/SUM(F$2:F$101)</f>
+      <c r="G64" s="5">
+        <f t="shared" si="3"/>
         <v>1.3551146529822545E-2</v>
       </c>
     </row>
@@ -3490,8 +3499,8 @@
       <c r="C65" s="3">
         <v>10642</v>
       </c>
-      <c r="D65" s="6">
-        <f>C65/SUM(C$2:C$101)</f>
+      <c r="D65" s="5">
+        <f t="shared" si="2"/>
         <v>3.8550442504163137E-3</v>
       </c>
       <c r="E65" s="3">
@@ -3500,8 +3509,8 @@
       <c r="F65" s="3">
         <v>23913472</v>
       </c>
-      <c r="G65" s="6">
-        <f>F65/SUM(F$2:F$101)</f>
+      <c r="G65" s="5">
+        <f t="shared" si="3"/>
         <v>8.6689474020256382E-3</v>
       </c>
     </row>
@@ -3515,8 +3524,8 @@
       <c r="C66" s="3">
         <v>10539</v>
       </c>
-      <c r="D66" s="6">
-        <f>C66/SUM(C$2:C$101)</f>
+      <c r="D66" s="5">
+        <f t="shared" ref="D66:D97" si="4">C66/SUM(C$2:C$101)</f>
         <v>3.8177326964045789E-3</v>
       </c>
       <c r="E66" s="3">
@@ -3525,8 +3534,8 @@
       <c r="F66" s="3">
         <v>32959488</v>
       </c>
-      <c r="G66" s="6">
-        <f>F66/SUM(F$2:F$101)</f>
+      <c r="G66" s="5">
+        <f t="shared" ref="G66:G97" si="5">F66/SUM(F$2:F$101)</f>
         <v>1.1948246907420853E-2</v>
       </c>
     </row>
@@ -3540,8 +3549,8 @@
       <c r="C67" s="3">
         <v>10117</v>
       </c>
-      <c r="D67" s="6">
-        <f>C67/SUM(C$2:C$101)</f>
+      <c r="D67" s="5">
+        <f t="shared" si="4"/>
         <v>3.6648639993856272E-3</v>
       </c>
       <c r="E67" s="3">
@@ -3550,8 +3559,8 @@
       <c r="F67" s="3">
         <v>78310400</v>
       </c>
-      <c r="G67" s="6">
-        <f>F67/SUM(F$2:F$101)</f>
+      <c r="G67" s="5">
+        <f t="shared" si="5"/>
         <v>2.8388547620002168E-2</v>
       </c>
     </row>
@@ -3565,8 +3574,8 @@
       <c r="C68" s="3">
         <v>9115</v>
       </c>
-      <c r="D68" s="6">
-        <f>C68/SUM(C$2:C$101)</f>
+      <c r="D68" s="5">
+        <f t="shared" si="4"/>
         <v>3.301891405989917E-3</v>
       </c>
       <c r="E68" s="3">
@@ -3575,8 +3584,8 @@
       <c r="F68" s="3">
         <v>32041984</v>
       </c>
-      <c r="G68" s="6">
-        <f>F68/SUM(F$2:F$101)</f>
+      <c r="G68" s="5">
+        <f t="shared" si="5"/>
         <v>1.1615639667570942E-2</v>
       </c>
     </row>
@@ -3590,8 +3599,8 @@
       <c r="C69" s="3">
         <v>8771</v>
       </c>
-      <c r="D69" s="6">
-        <f>C69/SUM(C$2:C$101)</f>
+      <c r="D69" s="5">
+        <f t="shared" si="4"/>
         <v>3.1772780605526674E-3</v>
       </c>
       <c r="E69" s="3">
@@ -3600,8 +3609,8 @@
       <c r="F69" s="3">
         <v>35514368</v>
       </c>
-      <c r="G69" s="6">
-        <f>F69/SUM(F$2:F$101)</f>
+      <c r="G69" s="5">
+        <f t="shared" si="5"/>
         <v>1.2874424433565417E-2</v>
       </c>
     </row>
@@ -3615,8 +3624,8 @@
       <c r="C70" s="3">
         <v>8646</v>
       </c>
-      <c r="D70" s="6">
-        <f>C70/SUM(C$2:C$101)</f>
+      <c r="D70" s="5">
+        <f t="shared" si="4"/>
         <v>3.1319970484025039E-3</v>
       </c>
       <c r="E70" s="3">
@@ -3625,8 +3634,8 @@
       <c r="F70" s="3">
         <v>8155136</v>
       </c>
-      <c r="G70" s="6">
-        <f>F70/SUM(F$2:F$101)</f>
+      <c r="G70" s="5">
+        <f t="shared" si="5"/>
         <v>2.95634381491595E-3</v>
       </c>
     </row>
@@ -3640,8 +3649,8 @@
       <c r="C71" s="3">
         <v>8376</v>
       </c>
-      <c r="D71" s="6">
-        <f>C71/SUM(C$2:C$101)</f>
+      <c r="D71" s="5">
+        <f t="shared" si="4"/>
         <v>3.034190062158151E-3</v>
       </c>
       <c r="E71" s="3">
@@ -3650,8 +3659,8 @@
       <c r="F71" s="3">
         <v>7703552</v>
       </c>
-      <c r="G71" s="6">
-        <f>F71/SUM(F$2:F$101)</f>
+      <c r="G71" s="5">
+        <f t="shared" si="5"/>
         <v>2.7926386890523218E-3</v>
       </c>
     </row>
@@ -3665,8 +3674,8 @@
       <c r="C72" s="3">
         <v>8298</v>
       </c>
-      <c r="D72" s="6">
-        <f>C72/SUM(C$2:C$101)</f>
+      <c r="D72" s="5">
+        <f t="shared" si="4"/>
         <v>3.0059347105764488E-3</v>
       </c>
       <c r="E72" s="3">
@@ -3675,8 +3684,8 @@
       <c r="F72" s="3">
         <v>22278144</v>
       </c>
-      <c r="G72" s="6">
-        <f>F72/SUM(F$2:F$101)</f>
+      <c r="G72" s="5">
+        <f t="shared" si="5"/>
         <v>8.076119542605651E-3</v>
       </c>
     </row>
@@ -3690,8 +3699,8 @@
       <c r="C73" s="3">
         <v>7762</v>
       </c>
-      <c r="D73" s="6">
-        <f>C73/SUM(C$2:C$101)</f>
+      <c r="D73" s="5">
+        <f t="shared" si="4"/>
         <v>2.8117697304765482E-3</v>
       </c>
       <c r="E73" s="3">
@@ -3700,8 +3709,8 @@
       <c r="F73" s="3">
         <v>572416</v>
       </c>
-      <c r="G73" s="6">
-        <f>F73/SUM(F$2:F$101)</f>
+      <c r="G73" s="5">
+        <f t="shared" si="5"/>
         <v>2.0750831146886187E-4</v>
       </c>
     </row>
@@ -3715,8 +3724,8 @@
       <c r="C74" s="3">
         <v>7521</v>
       </c>
-      <c r="D74" s="6">
-        <f>C74/SUM(C$2:C$101)</f>
+      <c r="D74" s="5">
+        <f t="shared" si="4"/>
         <v>2.7244679390510331E-3</v>
       </c>
       <c r="E74" s="3">
@@ -3725,8 +3734,8 @@
       <c r="F74" s="3">
         <v>80291840</v>
       </c>
-      <c r="G74" s="6">
-        <f>F74/SUM(F$2:F$101)</f>
+      <c r="G74" s="5">
+        <f t="shared" si="5"/>
         <v>2.9106845621240537E-2</v>
       </c>
     </row>
@@ -3740,8 +3749,8 @@
       <c r="C75" s="3">
         <v>7082</v>
       </c>
-      <c r="D75" s="6">
-        <f>C75/SUM(C$2:C$101)</f>
+      <c r="D75" s="5">
+        <f t="shared" si="4"/>
         <v>2.5654410243796592E-3</v>
       </c>
       <c r="E75" s="3">
@@ -3750,8 +3759,8 @@
       <c r="F75" s="3">
         <v>14179328</v>
       </c>
-      <c r="G75" s="6">
-        <f>F75/SUM(F$2:F$101)</f>
+      <c r="G75" s="5">
+        <f t="shared" si="5"/>
         <v>5.140192466742988E-3</v>
       </c>
     </row>
@@ -3765,8 +3774,8 @@
       <c r="C76" s="3">
         <v>6868</v>
       </c>
-      <c r="D76" s="6">
-        <f>C76/SUM(C$2:C$101)</f>
+      <c r="D76" s="5">
+        <f t="shared" si="4"/>
         <v>2.4879199315785794E-3</v>
       </c>
       <c r="E76" s="3">
@@ -3775,8 +3784,8 @@
       <c r="F76" s="3">
         <v>18896896</v>
       </c>
-      <c r="G76" s="6">
-        <f>F76/SUM(F$2:F$101)</f>
+      <c r="G76" s="5">
+        <f t="shared" si="5"/>
         <v>6.8503727725337691E-3</v>
       </c>
     </row>
@@ -3790,8 +3799,8 @@
       <c r="C77" s="3">
         <v>6164</v>
       </c>
-      <c r="D77" s="6">
-        <f>C77/SUM(C$2:C$101)</f>
+      <c r="D77" s="5">
+        <f t="shared" si="4"/>
         <v>2.2328972711488592E-3</v>
       </c>
       <c r="E77" s="3">
@@ -3800,8 +3809,8 @@
       <c r="F77" s="3">
         <v>430080</v>
       </c>
-      <c r="G77" s="6">
-        <f>F77/SUM(F$2:F$101)</f>
+      <c r="G77" s="5">
+        <f t="shared" si="5"/>
         <v>1.5590964367964577E-4</v>
       </c>
     </row>
@@ -3815,8 +3824,8 @@
       <c r="C78" s="3">
         <v>5911</v>
       </c>
-      <c r="D78" s="6">
-        <f>C78/SUM(C$2:C$101)</f>
+      <c r="D78" s="5">
+        <f t="shared" si="4"/>
         <v>2.141248502556928E-3</v>
       </c>
       <c r="E78" s="3">
@@ -3825,8 +3834,8 @@
       <c r="F78" s="3">
         <v>5855232</v>
       </c>
-      <c r="G78" s="6">
-        <f>F78/SUM(F$2:F$101)</f>
+      <c r="G78" s="5">
+        <f t="shared" si="5"/>
         <v>2.1225984346671775E-3</v>
       </c>
     </row>
@@ -3840,8 +3849,8 @@
       <c r="C79" s="3">
         <v>5638</v>
       </c>
-      <c r="D79" s="6">
-        <f>C79/SUM(C$2:C$101)</f>
+      <c r="D79" s="5">
+        <f t="shared" si="4"/>
         <v>2.0423547720209712E-3</v>
       </c>
       <c r="E79" s="3">
@@ -3850,8 +3859,8 @@
       <c r="F79" s="3">
         <v>10807296</v>
       </c>
-      <c r="G79" s="6">
-        <f>F79/SUM(F$2:F$101)</f>
+      <c r="G79" s="5">
+        <f t="shared" si="5"/>
         <v>3.9177866176070986E-3</v>
       </c>
     </row>
@@ -3865,8 +3874,8 @@
       <c r="C80" s="3">
         <v>5538</v>
       </c>
-      <c r="D80" s="6">
-        <f>C80/SUM(C$2:C$101)</f>
+      <c r="D80" s="5">
+        <f t="shared" si="4"/>
         <v>2.0061299623008407E-3</v>
       </c>
       <c r="E80" s="3">
@@ -3875,8 +3884,8 @@
       <c r="F80" s="3">
         <v>51678208</v>
       </c>
-      <c r="G80" s="6">
-        <f>F80/SUM(F$2:F$101)</f>
+      <c r="G80" s="5">
+        <f t="shared" si="5"/>
         <v>1.8734028541858769E-2</v>
       </c>
     </row>
@@ -3890,8 +3899,8 @@
       <c r="C81" s="3">
         <v>5487</v>
       </c>
-      <c r="D81" s="6">
-        <f>C81/SUM(C$2:C$101)</f>
+      <c r="D81" s="5">
+        <f t="shared" si="4"/>
         <v>1.9876553093435738E-3</v>
       </c>
       <c r="E81" s="3">
@@ -3900,8 +3909,8 @@
       <c r="F81" s="3">
         <v>1991680</v>
       </c>
-      <c r="G81" s="6">
-        <f>F81/SUM(F$2:F$101)</f>
+      <c r="G81" s="5">
+        <f t="shared" si="5"/>
         <v>7.2201013561169292E-4</v>
       </c>
     </row>
@@ -3915,8 +3924,8 @@
       <c r="C82" s="3">
         <v>5271</v>
       </c>
-      <c r="D82" s="6">
-        <f>C82/SUM(C$2:C$101)</f>
+      <c r="D82" s="5">
+        <f t="shared" si="4"/>
         <v>1.9094097203480914E-3</v>
       </c>
       <c r="E82" s="3">
@@ -3925,8 +3934,8 @@
       <c r="F82" s="3">
         <v>44034048</v>
       </c>
-      <c r="G82" s="6">
-        <f>F82/SUM(F$2:F$101)</f>
+      <c r="G82" s="5">
+        <f t="shared" si="5"/>
         <v>1.5962920232171732E-2</v>
       </c>
     </row>
@@ -3940,8 +3949,8 @@
       <c r="C83" s="3">
         <v>5249</v>
       </c>
-      <c r="D83" s="6">
-        <f>C83/SUM(C$2:C$101)</f>
+      <c r="D83" s="5">
+        <f t="shared" si="4"/>
         <v>1.9014402622096627E-3</v>
       </c>
       <c r="E83" s="3">
@@ -3950,8 +3959,8 @@
       <c r="F83" s="3">
         <v>15721472</v>
       </c>
-      <c r="G83" s="6">
-        <f>F83/SUM(F$2:F$101)</f>
+      <c r="G83" s="5">
+        <f t="shared" si="5"/>
         <v>5.6992399033657182E-3</v>
       </c>
     </row>
@@ -3965,8 +3974,8 @@
       <c r="C84" s="3">
         <v>5090</v>
       </c>
-      <c r="D84" s="6">
-        <f>C84/SUM(C$2:C$101)</f>
+      <c r="D84" s="5">
+        <f t="shared" si="4"/>
         <v>1.8438428147546549E-3</v>
       </c>
       <c r="E84" s="3">
@@ -3975,8 +3984,8 @@
       <c r="F84" s="3">
         <v>6299648</v>
       </c>
-      <c r="G84" s="6">
-        <f>F84/SUM(F$2:F$101)</f>
+      <c r="G84" s="5">
+        <f t="shared" si="5"/>
         <v>2.2837050664694779E-3</v>
       </c>
     </row>
@@ -3990,8 +3999,8 @@
       <c r="C85" s="3">
         <v>4448</v>
       </c>
-      <c r="D85" s="6">
-        <f>C85/SUM(C$2:C$101)</f>
+      <c r="D85" s="5">
+        <f t="shared" si="4"/>
         <v>1.6112795363514155E-3</v>
       </c>
       <c r="E85" s="3">
@@ -4000,8 +4009,8 @@
       <c r="F85" s="3">
         <v>1456128</v>
       </c>
-      <c r="G85" s="6">
-        <f>F85/SUM(F$2:F$101)</f>
+      <c r="G85" s="5">
+        <f t="shared" si="5"/>
         <v>5.2786550788680073E-4</v>
       </c>
     </row>
@@ -4015,8 +4024,8 @@
       <c r="C86" s="3">
         <v>3847</v>
       </c>
-      <c r="D86" s="6">
-        <f>C86/SUM(C$2:C$101)</f>
+      <c r="D86" s="5">
+        <f t="shared" si="4"/>
         <v>1.3935684299334298E-3</v>
       </c>
       <c r="E86" s="3">
@@ -4025,8 +4034,8 @@
       <c r="F86" s="3">
         <v>63996928</v>
       </c>
-      <c r="G86" s="6">
-        <f>F86/SUM(F$2:F$101)</f>
+      <c r="G86" s="5">
+        <f t="shared" si="5"/>
         <v>2.3199726192968624E-2</v>
       </c>
     </row>
@@ -4040,8 +4049,8 @@
       <c r="C87" s="3">
         <v>3541</v>
       </c>
-      <c r="D87" s="6">
-        <f>C87/SUM(C$2:C$101)</f>
+      <c r="D87" s="5">
+        <f t="shared" si="4"/>
         <v>1.2827205121898296E-3</v>
       </c>
       <c r="E87" s="3">
@@ -4050,8 +4059,8 @@
       <c r="F87" s="3">
         <v>54725632</v>
       </c>
-      <c r="G87" s="6">
-        <f>F87/SUM(F$2:F$101)</f>
+      <c r="G87" s="5">
+        <f t="shared" si="5"/>
         <v>1.9838759731360258E-2</v>
       </c>
     </row>
@@ -4065,8 +4074,8 @@
       <c r="C88" s="3">
         <v>3541</v>
       </c>
-      <c r="D88" s="6">
-        <f>C88/SUM(C$2:C$101)</f>
+      <c r="D88" s="5">
+        <f t="shared" si="4"/>
         <v>1.2827205121898296E-3</v>
       </c>
       <c r="E88" s="3">
@@ -4075,8 +4084,8 @@
       <c r="F88" s="3">
         <v>31309824</v>
       </c>
-      <c r="G88" s="6">
-        <f>F88/SUM(F$2:F$101)</f>
+      <c r="G88" s="5">
+        <f t="shared" si="5"/>
         <v>1.1350222059878212E-2</v>
       </c>
     </row>
@@ -4090,8 +4099,8 @@
       <c r="C89" s="3">
         <v>3294</v>
       </c>
-      <c r="D89" s="6">
-        <f>C89/SUM(C$2:C$101)</f>
+      <c r="D89" s="5">
+        <f t="shared" si="4"/>
         <v>1.1932452321811067E-3</v>
       </c>
       <c r="E89" s="3">
@@ -4100,8 +4109,8 @@
       <c r="F89" s="3">
         <v>9091072</v>
       </c>
-      <c r="G89" s="6">
-        <f>F89/SUM(F$2:F$101)</f>
+      <c r="G89" s="5">
+        <f t="shared" si="5"/>
         <v>3.2956328966378457E-3</v>
       </c>
     </row>
@@ -4115,8 +4124,8 @@
       <c r="C90" s="3">
         <v>2941</v>
       </c>
-      <c r="D90" s="6">
-        <f>C90/SUM(C$2:C$101)</f>
+      <c r="D90" s="5">
+        <f t="shared" si="4"/>
         <v>1.0653716538690451E-3</v>
       </c>
       <c r="E90" s="3">
@@ -4125,8 +4134,8 @@
       <c r="F90" s="3">
         <v>25308160</v>
       </c>
-      <c r="G90" s="6">
-        <f>F90/SUM(F$2:F$101)</f>
+      <c r="G90" s="5">
+        <f t="shared" si="5"/>
         <v>9.1745401036724891E-3</v>
       </c>
     </row>
@@ -4140,8 +4149,8 @@
       <c r="C91" s="3">
         <v>2726</v>
       </c>
-      <c r="D91" s="6">
-        <f>C91/SUM(C$2:C$101)</f>
+      <c r="D91" s="5">
+        <f t="shared" si="4"/>
         <v>9.8748831297076401E-4</v>
       </c>
       <c r="E91" s="3">
@@ -4150,8 +4159,8 @@
       <c r="F91" s="3">
         <v>3296256</v>
       </c>
-      <c r="G91" s="6">
-        <f>F91/SUM(F$2:F$101)</f>
+      <c r="G91" s="5">
+        <f t="shared" si="5"/>
         <v>1.194936054773285E-3</v>
       </c>
     </row>
@@ -4165,8 +4174,8 @@
       <c r="C92" s="3">
         <v>2480</v>
       </c>
-      <c r="D92" s="6">
-        <f>C92/SUM(C$2:C$101)</f>
+      <c r="D92" s="5">
+        <f t="shared" si="4"/>
         <v>8.9837528105924237E-4</v>
       </c>
       <c r="E92" s="3">
@@ -4175,8 +4184,8 @@
       <c r="F92" s="3">
         <v>8670208</v>
       </c>
-      <c r="G92" s="6">
-        <f>F92/SUM(F$2:F$101)</f>
+      <c r="G92" s="5">
+        <f t="shared" si="5"/>
         <v>3.1430641738941921E-3</v>
       </c>
     </row>
@@ -4190,8 +4199,8 @@
       <c r="C93" s="3">
         <v>1988</v>
       </c>
-      <c r="D93" s="6">
-        <f>C93/SUM(C$2:C$101)</f>
+      <c r="D93" s="5">
+        <f t="shared" si="4"/>
         <v>7.201492172361992E-4</v>
       </c>
       <c r="E93" s="3">
@@ -4200,8 +4209,8 @@
       <c r="F93" s="3">
         <v>91447296</v>
       </c>
-      <c r="G93" s="6">
-        <f>F93/SUM(F$2:F$101)</f>
+      <c r="G93" s="5">
+        <f t="shared" si="5"/>
         <v>3.3150844807540679E-2</v>
       </c>
     </row>
@@ -4215,8 +4224,8 @@
       <c r="C94" s="3">
         <v>1925</v>
       </c>
-      <c r="D94" s="6">
-        <f>C94/SUM(C$2:C$101)</f>
+      <c r="D94" s="5">
+        <f t="shared" si="4"/>
         <v>6.9732758711251678E-4</v>
       </c>
       <c r="E94" s="3">
@@ -4225,8 +4234,8 @@
       <c r="F94" s="3">
         <v>54236160</v>
       </c>
-      <c r="G94" s="6">
-        <f>F94/SUM(F$2:F$101)</f>
+      <c r="G94" s="5">
+        <f t="shared" si="5"/>
         <v>1.966131970831533E-2</v>
       </c>
     </row>
@@ -4240,8 +4249,8 @@
       <c r="C95" s="3">
         <v>1845</v>
       </c>
-      <c r="D95" s="6">
-        <f>C95/SUM(C$2:C$101)</f>
+      <c r="D95" s="5">
+        <f t="shared" si="4"/>
         <v>6.683477393364122E-4</v>
       </c>
       <c r="E95" s="3">
@@ -4250,8 +4259,8 @@
       <c r="F95" s="3">
         <v>22433792</v>
       </c>
-      <c r="G95" s="6">
-        <f>F95/SUM(F$2:F$101)</f>
+      <c r="G95" s="5">
+        <f t="shared" si="5"/>
         <v>8.1325439850801901E-3</v>
       </c>
     </row>
@@ -4265,8 +4274,8 @@
       <c r="C96" s="3">
         <v>1518</v>
       </c>
-      <c r="D96" s="6">
-        <f>C96/SUM(C$2:C$101)</f>
+      <c r="D96" s="5">
+        <f t="shared" si="4"/>
         <v>5.4989261155158472E-4</v>
       </c>
       <c r="E96" s="3">
@@ -4275,8 +4284,8 @@
       <c r="F96" s="3">
         <v>5821440</v>
       </c>
-      <c r="G96" s="6">
-        <f>F96/SUM(F$2:F$101)</f>
+      <c r="G96" s="5">
+        <f t="shared" si="5"/>
         <v>2.1103483912352054E-3</v>
       </c>
     </row>
@@ -4290,8 +4299,8 @@
       <c r="C97" s="3">
         <v>618</v>
       </c>
-      <c r="D97" s="6">
-        <f>C97/SUM(C$2:C$101)</f>
+      <c r="D97" s="5">
+        <f t="shared" si="4"/>
         <v>2.2386932407040798E-4</v>
       </c>
       <c r="E97" s="3">
@@ -4300,8 +4309,8 @@
       <c r="F97" s="3">
         <v>557056</v>
       </c>
-      <c r="G97" s="6">
-        <f>F97/SUM(F$2:F$101)</f>
+      <c r="G97" s="5">
+        <f t="shared" si="5"/>
         <v>2.0194010990887452E-4</v>
       </c>
     </row>
@@ -4315,8 +4324,8 @@
       <c r="C98" s="3">
         <v>329</v>
       </c>
-      <c r="D98" s="6">
-        <f>C98/SUM(C$2:C$101)</f>
+      <c r="D98" s="5">
+        <f t="shared" ref="D98:D101" si="6">C98/SUM(C$2:C$101)</f>
         <v>1.1917962397923015E-4</v>
       </c>
       <c r="E98" s="3">
@@ -4325,8 +4334,8 @@
       <c r="F98" s="3">
         <v>45967360</v>
       </c>
-      <c r="G98" s="6">
-        <f>F98/SUM(F$2:F$101)</f>
+      <c r="G98" s="5">
+        <f t="shared" ref="G98:G101" si="7">F98/SUM(F$2:F$101)</f>
         <v>1.6663771201855474E-2</v>
       </c>
     </row>
@@ -4340,8 +4349,8 @@
       <c r="C99" s="3">
         <v>255</v>
       </c>
-      <c r="D99" s="6">
-        <f>C99/SUM(C$2:C$101)</f>
+      <c r="D99" s="5">
+        <f t="shared" si="6"/>
         <v>9.2373264786333394E-5</v>
       </c>
       <c r="E99" s="3">
@@ -4350,8 +4359,8 @@
       <c r="F99" s="3">
         <v>39258112</v>
       </c>
-      <c r="G99" s="6">
-        <f>F99/SUM(F$2:F$101)</f>
+      <c r="G99" s="5">
+        <f t="shared" si="7"/>
         <v>1.4231580760453E-2</v>
       </c>
     </row>
@@ -4365,8 +4374,8 @@
       <c r="C100" s="3">
         <v>226</v>
       </c>
-      <c r="D100" s="6">
-        <f>C100/SUM(C$2:C$101)</f>
+      <c r="D100" s="5">
+        <f t="shared" si="6"/>
         <v>8.1868069967495484E-5</v>
       </c>
       <c r="E100" s="3">
@@ -4375,8 +4384,8 @@
       <c r="F100" s="3">
         <v>41382912</v>
       </c>
-      <c r="G100" s="6">
-        <f>F100/SUM(F$2:F$101)</f>
+      <c r="G100" s="5">
+        <f t="shared" si="7"/>
         <v>1.5001848642917915E-2</v>
       </c>
     </row>
@@ -4390,8 +4399,8 @@
       <c r="C101" s="3">
         <v>9</v>
       </c>
-      <c r="D101" s="6">
-        <f>C101/SUM(C$2:C$101)</f>
+      <c r="D101" s="5">
+        <f t="shared" si="6"/>
         <v>3.2602328748117669E-6</v>
       </c>
       <c r="E101" s="3">
@@ -4400,12 +4409,13 @@
       <c r="F101" s="3">
         <v>9145344</v>
       </c>
-      <c r="G101" s="6">
-        <f>F101/SUM(F$2:F$101)</f>
+      <c r="G101" s="5">
+        <f t="shared" si="7"/>
         <v>3.3153072088164676E-3</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <sortState ref="A2:G101">
     <sortCondition descending="1" ref="C2:C101"/>
     <sortCondition ref="A2:A101"/>
@@ -4570,6 +4580,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <sortState ref="A2:D10">
     <sortCondition descending="1" ref="C2:C10"/>
     <sortCondition ref="B2:B10"/>
@@ -4596,14 +4607,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
     </row>
     <row r="2" spans="1:6" ht="15.75">
       <c r="A2" s="1" t="s">
@@ -4638,10 +4649,10 @@
       <c r="D3" s="3">
         <v>90707</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="4">
         <v>84.814453125</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="5">
         <f>C3/$C$13</f>
         <v>2.3739204553893278E-2</v>
       </c>
@@ -4659,10 +4670,10 @@
       <c r="D4" s="3">
         <v>6745</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <v>44.9033203125</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="5">
         <f t="shared" ref="F4:F12" si="0">C4/$C$13</f>
         <v>2.392503782775755E-2</v>
       </c>
@@ -4680,10 +4691,10 @@
       <c r="D5" s="3">
         <v>42413</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <v>18.833984375</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="5">
         <f t="shared" si="0"/>
         <v>2.4426751442381361E-2</v>
       </c>
@@ -4701,10 +4712,10 @@
       <c r="D6" s="3">
         <v>7964</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="4">
         <v>78.3671875</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="5">
         <f t="shared" si="0"/>
         <v>2.5940586240585626E-2</v>
       </c>
@@ -4722,10 +4733,10 @@
       <c r="D7" s="3">
         <v>21381</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="4">
         <v>26.0166015625</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="5">
         <f t="shared" si="0"/>
         <v>2.6592632815547978E-2</v>
       </c>
@@ -4743,10 +4754,10 @@
       <c r="D8" s="3">
         <v>10968</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="4">
         <v>13.021484375</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="5">
         <f t="shared" si="0"/>
         <v>2.6920829591612364E-2</v>
       </c>
@@ -4764,10 +4775,10 @@
       <c r="D9" s="3">
         <v>6108</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="4">
         <v>0.4189453125</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="5">
         <f t="shared" si="0"/>
         <v>2.8375980198070014E-2</v>
       </c>
@@ -4785,10 +4796,10 @@
       <c r="D10" s="3">
         <v>30001</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="4">
         <v>8.529296875</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="5">
         <f t="shared" si="0"/>
         <v>2.9064251582752498E-2</v>
       </c>
@@ -4806,10 +4817,10 @@
       <c r="D11" s="3">
         <v>5016</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="4">
         <v>34.2744140625</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="5">
         <f t="shared" si="0"/>
         <v>3.2342959110521534E-2</v>
       </c>
@@ -4827,17 +4838,17 @@
       <c r="D12" s="3">
         <v>17813</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="4">
         <v>20.2607421875</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="5">
         <f t="shared" si="0"/>
         <v>3.289719869923953E-2</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="C13" s="3">
         <f>SUM(FrequencyReport!C2:C101)</f>
@@ -4847,20 +4858,20 @@
         <f>SUM(FrequencyReport!E2:E101)</f>
         <v>2728933</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="4">
         <f>SUM(FrequencyReport!F2:F101)/1024/1024</f>
         <v>2630.73046875</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="6" t="s">
         <v>225</v>
       </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
     </row>
     <row r="15" spans="1:6" ht="15.75">
       <c r="A15" s="1" t="s">
@@ -4895,10 +4906,10 @@
       <c r="D16" s="3">
         <v>15029</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="4">
         <v>56.8212890625</v>
       </c>
-      <c r="F16" s="6">
+      <c r="F16" s="5">
         <f>E16/$E$26</f>
         <v>2.1599053851190927E-2</v>
       </c>
@@ -4916,10 +4927,10 @@
       <c r="D17" s="3">
         <v>40501</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="4">
         <v>58.2158203125</v>
       </c>
-      <c r="F17" s="6">
+      <c r="F17" s="5">
         <f t="shared" ref="F17:F25" si="1">E17/$E$26</f>
         <v>2.2129146639701721E-2</v>
       </c>
@@ -4937,10 +4948,10 @@
       <c r="D18" s="3">
         <v>11091</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E18" s="4">
         <v>61.0322265625</v>
       </c>
-      <c r="F18" s="6">
+      <c r="F18" s="5">
         <f t="shared" si="1"/>
         <v>2.3199726192968624E-2</v>
       </c>
@@ -4958,10 +4969,10 @@
       <c r="D19" s="3">
         <v>63556</v>
       </c>
-      <c r="E19" s="5">
+      <c r="E19" s="4">
         <v>63.0126953125</v>
       </c>
-      <c r="F19" s="6">
+      <c r="F19" s="5">
         <f t="shared" si="1"/>
         <v>2.3952547043878912E-2</v>
       </c>
@@ -4979,10 +4990,10 @@
       <c r="D20" s="3">
         <v>48496</v>
       </c>
-      <c r="E20" s="5">
+      <c r="E20" s="4">
         <v>74.6826171875</v>
       </c>
-      <c r="F20" s="6">
+      <c r="F20" s="5">
         <f t="shared" si="1"/>
         <v>2.8388547620002168E-2</v>
       </c>
@@ -5000,10 +5011,10 @@
       <c r="D21" s="3">
         <v>27035</v>
       </c>
-      <c r="E21" s="5">
+      <c r="E21" s="4">
         <v>76.572265625</v>
       </c>
-      <c r="F21" s="6">
+      <c r="F21" s="5">
         <f t="shared" si="1"/>
         <v>2.9106845621240537E-2</v>
       </c>
@@ -5021,10 +5032,10 @@
       <c r="D22" s="3">
         <v>7964</v>
       </c>
-      <c r="E22" s="5">
+      <c r="E22" s="4">
         <v>78.3671875</v>
       </c>
-      <c r="F22" s="6">
+      <c r="F22" s="5">
         <f t="shared" si="1"/>
         <v>2.9789135919057651E-2</v>
       </c>
@@ -5042,10 +5053,10 @@
       <c r="D23" s="3">
         <v>90707</v>
       </c>
-      <c r="E23" s="5">
+      <c r="E23" s="4">
         <v>84.814453125</v>
       </c>
-      <c r="F23" s="6">
+      <c r="F23" s="5">
         <f t="shared" si="1"/>
         <v>3.2239887032326754E-2</v>
       </c>
@@ -5063,10 +5074,10 @@
       <c r="D24" s="3">
         <v>39951</v>
       </c>
-      <c r="E24" s="5">
+      <c r="E24" s="4">
         <v>87.2109375</v>
       </c>
-      <c r="F24" s="6">
+      <c r="F24" s="5">
         <f t="shared" si="1"/>
         <v>3.3150844807540679E-2</v>
       </c>
@@ -5084,17 +5095,17 @@
       <c r="D25" s="3">
         <v>7635</v>
       </c>
-      <c r="E25" s="5">
+      <c r="E25" s="4">
         <v>92.1328125</v>
       </c>
-      <c r="F25" s="6">
+      <c r="F25" s="5">
         <f t="shared" si="1"/>
         <v>3.5021760531696429E-2</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="C26" s="3">
         <f>SUM(FrequencyReport!C2:C101)</f>
@@ -5104,20 +5115,20 @@
         <f>SUM(FrequencyReport!E2:E101)</f>
         <v>2728933</v>
       </c>
-      <c r="E26" s="5">
+      <c r="E26" s="4">
         <f>SUM(FrequencyReport!F2:F101)/1024/1024</f>
         <v>2630.73046875</v>
       </c>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
+      <c r="A27" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
     </row>
     <row r="28" spans="1:6" ht="15.75">
       <c r="A28" s="1" t="s">
@@ -5264,14 +5275,18 @@
       </c>
     </row>
     <row r="38" spans="1:4">
+      <c r="A38" t="s">
+        <v>233</v>
+      </c>
       <c r="D38" s="3">
         <f>SUM(DataCategories!D2:D10)</f>
         <v>3565130636</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A15:E24">
-    <sortCondition ref="E15:E24"/>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <sortState ref="A29:D37">
+    <sortCondition descending="1" ref="C29:C37"/>
   </sortState>
   <mergeCells count="3">
     <mergeCell ref="A14:F14"/>

</xml_diff>